<commit_message>
openpyxl - criando uma planilha e inserindo dados com python
</commit_message>
<xml_diff>
--- a/AULA146_Openpyxl/planilha_modificada.xlsx
+++ b/AULA146_Openpyxl/planilha_modificada.xlsx
@@ -1,37 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjetosPython\Secao5-Modulos\AULA146_Openpyxl\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5A0DD9-C7EB-4C11-969D-DC7A807CA585}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Página1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>pedido</t>
+  </si>
+  <si>
+    <t>id_produto</t>
+  </si>
+  <si>
+    <t>preco</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$R$ -416]#,##0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -50,82 +70,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -425,210 +386,203 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col width="16.42578125" customWidth="1" min="1" max="1"/>
-    <col width="19.28515625" customWidth="1" min="3" max="4"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="3" max="4" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>pedido</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>id_produto</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>preco</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="n"/>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="n">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>1002</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="2">
         <v>50</v>
       </c>
-      <c r="D2" s="2" t="n"/>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="n">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="1">
         <v>1005</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="2">
         <v>32.25</v>
       </c>
-      <c r="D3" s="2" t="n"/>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="n">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="1">
         <v>1200</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>89.98999999999999</v>
-      </c>
-      <c r="D4" s="2" t="n"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="n">
+      <c r="C4" s="2">
+        <v>89.99</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="1">
         <v>1205</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="2">
         <v>68.42</v>
       </c>
-      <c r="D5" s="2" t="n"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="n">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="1">
         <v>1206</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="2">
         <v>28.73</v>
       </c>
-      <c r="D6" s="2" t="n"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="n">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="1">
         <v>1207</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="2">
         <v>60.67</v>
       </c>
-      <c r="D7" s="2" t="n"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="1" t="n">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="1">
         <v>1208</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="2">
         <v>37.43</v>
       </c>
-      <c r="D8" s="2" t="n"/>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="1" t="n">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="1">
         <v>1209</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="2">
         <v>42.51</v>
       </c>
-      <c r="D9" s="2" t="n"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="n">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="1">
         <v>1210</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="2">
         <v>52.07</v>
       </c>
-      <c r="D10" s="2" t="n"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="1" t="n">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="1">
         <v>1211</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="2">
         <v>38.31</v>
       </c>
-      <c r="D11" s="2" t="n"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="1" t="n">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="1">
         <v>1212</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" s="2">
         <v>58.11</v>
       </c>
-      <c r="D12" s="2" t="n"/>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="1" t="n">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="1">
         <v>1213</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" s="2">
         <v>90.05</v>
       </c>
-      <c r="D13" s="2" t="n"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="1" t="n">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="1">
         <v>1214</v>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="2">
         <v>30.96</v>
       </c>
-      <c r="D14" s="2" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>1215</v>
       </c>
-      <c r="C15" t="n">
-        <v>81.48999999999999</v>
+      <c r="C15">
+        <v>81.489999999999995</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>